<commit_message>
Heather comments and percent
</commit_message>
<xml_diff>
--- a/Period_week_summary.xlsx
+++ b/Period_week_summary.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C378"/>
+  <dimension ref="A1:D378"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,7 +446,12 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>only_one_adult_present</t>
+          <t>AM_Flying</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>AM_Flying_percent</t>
         </is>
       </c>
     </row>
@@ -462,6 +467,9 @@
       <c r="C2" t="n">
         <v>0</v>
       </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -475,6 +483,9 @@
       <c r="C3" t="n">
         <v>0</v>
       </c>
+      <c r="D3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -488,6 +499,9 @@
       <c r="C4" t="n">
         <v>0</v>
       </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -499,7 +513,10 @@
         <v>30</v>
       </c>
       <c r="C5" t="n">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="D5" t="n">
+        <v>3.333333333333333</v>
       </c>
     </row>
     <row r="6">
@@ -514,6 +531,9 @@
       <c r="C6" t="n">
         <v>0</v>
       </c>
+      <c r="D6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -527,6 +547,9 @@
       <c r="C7" t="n">
         <v>0</v>
       </c>
+      <c r="D7" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -540,6 +563,9 @@
       <c r="C8" t="n">
         <v>0</v>
       </c>
+      <c r="D8" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -553,6 +579,9 @@
       <c r="C9" t="n">
         <v>0</v>
       </c>
+      <c r="D9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -566,6 +595,9 @@
       <c r="C10" t="n">
         <v>0</v>
       </c>
+      <c r="D10" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -579,6 +611,9 @@
       <c r="C11" t="n">
         <v>0</v>
       </c>
+      <c r="D11" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -592,6 +627,9 @@
       <c r="C12" t="n">
         <v>0</v>
       </c>
+      <c r="D12" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -605,6 +643,9 @@
       <c r="C13" t="n">
         <v>0</v>
       </c>
+      <c r="D13" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -618,6 +659,9 @@
       <c r="C14" t="n">
         <v>0</v>
       </c>
+      <c r="D14" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -629,7 +673,10 @@
         <v>77</v>
       </c>
       <c r="C15" t="n">
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="D15" t="n">
+        <v>2.597402597402597</v>
       </c>
     </row>
     <row r="16">
@@ -642,7 +689,10 @@
         <v>51</v>
       </c>
       <c r="C16" t="n">
-        <v>0</v>
+        <v>9</v>
+      </c>
+      <c r="D16" t="n">
+        <v>5.88235294117647</v>
       </c>
     </row>
     <row r="17">
@@ -655,7 +705,10 @@
         <v>110</v>
       </c>
       <c r="C17" t="n">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0.9090909090909091</v>
       </c>
     </row>
     <row r="18">
@@ -668,7 +721,10 @@
         <v>42</v>
       </c>
       <c r="C18" t="n">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="D18" t="n">
+        <v>2.380952380952381</v>
       </c>
     </row>
     <row r="19">
@@ -683,6 +739,9 @@
       <c r="C19" t="n">
         <v>0</v>
       </c>
+      <c r="D19" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -696,6 +755,9 @@
       <c r="C20" t="n">
         <v>0</v>
       </c>
+      <c r="D20" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -707,7 +769,10 @@
         <v>145</v>
       </c>
       <c r="C21" t="n">
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="D21" t="n">
+        <v>1.379310344827586</v>
       </c>
     </row>
     <row r="22">
@@ -722,6 +787,9 @@
       <c r="C22" t="n">
         <v>0</v>
       </c>
+      <c r="D22" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -733,7 +801,10 @@
         <v>80</v>
       </c>
       <c r="C23" t="n">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="D23" t="n">
+        <v>1.25</v>
       </c>
     </row>
     <row r="24">
@@ -748,6 +819,9 @@
       <c r="C24" t="n">
         <v>0</v>
       </c>
+      <c r="D24" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -761,6 +835,9 @@
       <c r="C25" t="n">
         <v>0</v>
       </c>
+      <c r="D25" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -772,7 +849,10 @@
         <v>40</v>
       </c>
       <c r="C26" t="n">
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="D26" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="27">
@@ -787,6 +867,9 @@
       <c r="C27" t="n">
         <v>0</v>
       </c>
+      <c r="D27" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -800,6 +883,9 @@
       <c r="C28" t="n">
         <v>0</v>
       </c>
+      <c r="D28" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -813,6 +899,9 @@
       <c r="C29" t="n">
         <v>0</v>
       </c>
+      <c r="D29" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -824,7 +913,10 @@
         <v>60</v>
       </c>
       <c r="C30" t="n">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="D30" t="n">
+        <v>1.666666666666667</v>
       </c>
     </row>
     <row r="31">
@@ -839,6 +931,9 @@
       <c r="C31" t="n">
         <v>0</v>
       </c>
+      <c r="D31" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -852,6 +947,9 @@
       <c r="C32" t="n">
         <v>0</v>
       </c>
+      <c r="D32" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -863,7 +961,10 @@
         <v>67</v>
       </c>
       <c r="C33" t="n">
-        <v>0</v>
+        <v>9</v>
+      </c>
+      <c r="D33" t="n">
+        <v>4.477611940298507</v>
       </c>
     </row>
     <row r="34">
@@ -878,6 +979,9 @@
       <c r="C34" t="n">
         <v>0</v>
       </c>
+      <c r="D34" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -889,7 +993,10 @@
         <v>41</v>
       </c>
       <c r="C35" t="n">
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="D35" t="n">
+        <v>4.878048780487805</v>
       </c>
     </row>
     <row r="36">
@@ -902,7 +1009,10 @@
         <v>30</v>
       </c>
       <c r="C36" t="n">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="D36" t="n">
+        <v>3.333333333333333</v>
       </c>
     </row>
     <row r="37">
@@ -915,7 +1025,10 @@
         <v>30</v>
       </c>
       <c r="C37" t="n">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="D37" t="n">
+        <v>3.333333333333333</v>
       </c>
     </row>
     <row r="38">
@@ -928,7 +1041,10 @@
         <v>60</v>
       </c>
       <c r="C38" t="n">
-        <v>0</v>
+        <v>12</v>
+      </c>
+      <c r="D38" t="n">
+        <v>6.666666666666667</v>
       </c>
     </row>
     <row r="39">
@@ -943,6 +1059,9 @@
       <c r="C39" t="n">
         <v>0</v>
       </c>
+      <c r="D39" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -956,6 +1075,9 @@
       <c r="C40" t="n">
         <v>0</v>
       </c>
+      <c r="D40" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -967,7 +1089,10 @@
         <v>60</v>
       </c>
       <c r="C41" t="n">
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="D41" t="n">
+        <v>3.333333333333333</v>
       </c>
     </row>
     <row r="42">
@@ -980,7 +1105,10 @@
         <v>62</v>
       </c>
       <c r="C42" t="n">
-        <v>0</v>
+        <v>9</v>
+      </c>
+      <c r="D42" t="n">
+        <v>4.838709677419355</v>
       </c>
     </row>
     <row r="43">
@@ -993,7 +1121,10 @@
         <v>63</v>
       </c>
       <c r="C43" t="n">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="D43" t="n">
+        <v>1.587301587301587</v>
       </c>
     </row>
     <row r="44">
@@ -1006,7 +1137,10 @@
         <v>29</v>
       </c>
       <c r="C44" t="n">
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="D44" t="n">
+        <v>6.896551724137931</v>
       </c>
     </row>
     <row r="45">
@@ -1019,7 +1153,10 @@
         <v>80</v>
       </c>
       <c r="C45" t="n">
-        <v>0</v>
+        <v>15</v>
+      </c>
+      <c r="D45" t="n">
+        <v>6.25</v>
       </c>
     </row>
     <row r="46">
@@ -1034,6 +1171,9 @@
       <c r="C46" t="n">
         <v>0</v>
       </c>
+      <c r="D46" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -1045,7 +1185,10 @@
         <v>62</v>
       </c>
       <c r="C47" t="n">
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="D47" t="n">
+        <v>3.225806451612903</v>
       </c>
     </row>
     <row r="48">
@@ -1060,6 +1203,9 @@
       <c r="C48" t="n">
         <v>0</v>
       </c>
+      <c r="D48" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -1073,6 +1219,9 @@
       <c r="C49" t="n">
         <v>0</v>
       </c>
+      <c r="D49" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -1084,7 +1233,10 @@
         <v>96</v>
       </c>
       <c r="C50" t="n">
-        <v>0</v>
+        <v>21</v>
+      </c>
+      <c r="D50" t="n">
+        <v>7.291666666666667</v>
       </c>
     </row>
     <row r="51">
@@ -1097,7 +1249,10 @@
         <v>30</v>
       </c>
       <c r="C51" t="n">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="D51" t="n">
+        <v>3.333333333333333</v>
       </c>
     </row>
     <row r="52">
@@ -1112,6 +1267,9 @@
       <c r="C52" t="n">
         <v>0</v>
       </c>
+      <c r="D52" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -1123,7 +1281,10 @@
         <v>33</v>
       </c>
       <c r="C53" t="n">
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="D53" t="n">
+        <v>6.060606060606061</v>
       </c>
     </row>
     <row r="54">
@@ -1138,6 +1299,9 @@
       <c r="C54" t="n">
         <v>0</v>
       </c>
+      <c r="D54" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -1151,6 +1315,9 @@
       <c r="C55" t="n">
         <v>0</v>
       </c>
+      <c r="D55" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -1164,6 +1331,9 @@
       <c r="C56" t="n">
         <v>0</v>
       </c>
+      <c r="D56" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -1177,6 +1347,9 @@
       <c r="C57" t="n">
         <v>0</v>
       </c>
+      <c r="D57" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -1190,6 +1363,9 @@
       <c r="C58" t="n">
         <v>0</v>
       </c>
+      <c r="D58" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -1203,6 +1379,9 @@
       <c r="C59" t="n">
         <v>0</v>
       </c>
+      <c r="D59" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -1216,6 +1395,9 @@
       <c r="C60" t="n">
         <v>0</v>
       </c>
+      <c r="D60" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -1229,6 +1411,9 @@
       <c r="C61" t="n">
         <v>0</v>
       </c>
+      <c r="D61" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -1242,6 +1427,9 @@
       <c r="C62" t="n">
         <v>0</v>
       </c>
+      <c r="D62" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -1255,6 +1443,9 @@
       <c r="C63" t="n">
         <v>0</v>
       </c>
+      <c r="D63" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -1268,6 +1459,9 @@
       <c r="C64" t="n">
         <v>0</v>
       </c>
+      <c r="D64" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -1281,6 +1475,9 @@
       <c r="C65" t="n">
         <v>0</v>
       </c>
+      <c r="D65" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -1292,7 +1489,10 @@
         <v>31</v>
       </c>
       <c r="C66" t="n">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="D66" t="n">
+        <v>3.225806451612903</v>
       </c>
     </row>
     <row r="67">
@@ -1305,7 +1505,10 @@
         <v>30</v>
       </c>
       <c r="C67" t="n">
-        <v>0</v>
+        <v>9</v>
+      </c>
+      <c r="D67" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="68">
@@ -1320,6 +1523,9 @@
       <c r="C68" t="n">
         <v>0</v>
       </c>
+      <c r="D68" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -1331,7 +1537,10 @@
         <v>40</v>
       </c>
       <c r="C69" t="n">
-        <v>0</v>
+        <v>9</v>
+      </c>
+      <c r="D69" t="n">
+        <v>7.5</v>
       </c>
     </row>
     <row r="70">
@@ -1346,6 +1555,9 @@
       <c r="C70" t="n">
         <v>0</v>
       </c>
+      <c r="D70" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -1357,7 +1569,10 @@
         <v>36</v>
       </c>
       <c r="C71" t="n">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="D71" t="n">
+        <v>2.777777777777778</v>
       </c>
     </row>
     <row r="72">
@@ -1370,7 +1585,10 @@
         <v>40</v>
       </c>
       <c r="C72" t="n">
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="D72" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="73">
@@ -1383,7 +1601,10 @@
         <v>70</v>
       </c>
       <c r="C73" t="n">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="D73" t="n">
+        <v>1.428571428571429</v>
       </c>
     </row>
     <row r="74">
@@ -1398,6 +1619,9 @@
       <c r="C74" t="n">
         <v>0</v>
       </c>
+      <c r="D74" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -1411,6 +1635,9 @@
       <c r="C75" t="n">
         <v>0</v>
       </c>
+      <c r="D75" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -1422,7 +1649,10 @@
         <v>40</v>
       </c>
       <c r="C76" t="n">
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="D76" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="77">
@@ -1435,7 +1665,10 @@
         <v>40</v>
       </c>
       <c r="C77" t="n">
-        <v>0</v>
+        <v>9</v>
+      </c>
+      <c r="D77" t="n">
+        <v>7.5</v>
       </c>
     </row>
     <row r="78">
@@ -1448,7 +1681,10 @@
         <v>40</v>
       </c>
       <c r="C78" t="n">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="D78" t="n">
+        <v>2.5</v>
       </c>
     </row>
     <row r="79">
@@ -1463,6 +1699,9 @@
       <c r="C79" t="n">
         <v>0</v>
       </c>
+      <c r="D79" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -1476,6 +1715,9 @@
       <c r="C80" t="n">
         <v>0</v>
       </c>
+      <c r="D80" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -1489,6 +1731,9 @@
       <c r="C81" t="n">
         <v>0</v>
       </c>
+      <c r="D81" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -1502,6 +1747,9 @@
       <c r="C82" t="n">
         <v>0</v>
       </c>
+      <c r="D82" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -1513,7 +1761,10 @@
         <v>40</v>
       </c>
       <c r="C83" t="n">
-        <v>0</v>
+        <v>9</v>
+      </c>
+      <c r="D83" t="n">
+        <v>7.5</v>
       </c>
     </row>
     <row r="84">
@@ -1528,6 +1779,9 @@
       <c r="C84" t="n">
         <v>0</v>
       </c>
+      <c r="D84" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -1541,6 +1795,9 @@
       <c r="C85" t="n">
         <v>0</v>
       </c>
+      <c r="D85" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -1552,7 +1809,10 @@
         <v>40</v>
       </c>
       <c r="C86" t="n">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="D86" t="n">
+        <v>2.5</v>
       </c>
     </row>
     <row r="87">
@@ -1567,6 +1827,9 @@
       <c r="C87" t="n">
         <v>0</v>
       </c>
+      <c r="D87" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -1580,6 +1843,9 @@
       <c r="C88" t="n">
         <v>0</v>
       </c>
+      <c r="D88" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -1593,6 +1859,9 @@
       <c r="C89" t="n">
         <v>0</v>
       </c>
+      <c r="D89" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -1606,6 +1875,9 @@
       <c r="C90" t="n">
         <v>0</v>
       </c>
+      <c r="D90" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -1617,7 +1889,10 @@
         <v>125</v>
       </c>
       <c r="C91" t="n">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="D91" t="n">
+        <v>0.8</v>
       </c>
     </row>
     <row r="92">
@@ -1630,7 +1905,10 @@
         <v>121</v>
       </c>
       <c r="C92" t="n">
-        <v>0</v>
+        <v>9</v>
+      </c>
+      <c r="D92" t="n">
+        <v>2.479338842975207</v>
       </c>
     </row>
     <row r="93">
@@ -1643,7 +1921,10 @@
         <v>150</v>
       </c>
       <c r="C93" t="n">
-        <v>0</v>
+        <v>15</v>
+      </c>
+      <c r="D93" t="n">
+        <v>3.333333333333333</v>
       </c>
     </row>
     <row r="94">
@@ -1656,7 +1937,10 @@
         <v>188</v>
       </c>
       <c r="C94" t="n">
-        <v>0</v>
+        <v>12</v>
+      </c>
+      <c r="D94" t="n">
+        <v>2.127659574468085</v>
       </c>
     </row>
     <row r="95">
@@ -1669,7 +1953,10 @@
         <v>158</v>
       </c>
       <c r="C95" t="n">
-        <v>0</v>
+        <v>30</v>
+      </c>
+      <c r="D95" t="n">
+        <v>6.329113924050633</v>
       </c>
     </row>
     <row r="96">
@@ -1682,7 +1969,10 @@
         <v>207</v>
       </c>
       <c r="C96" t="n">
-        <v>0</v>
+        <v>18</v>
+      </c>
+      <c r="D96" t="n">
+        <v>2.898550724637681</v>
       </c>
     </row>
     <row r="97">
@@ -1695,7 +1985,10 @@
         <v>142</v>
       </c>
       <c r="C97" t="n">
-        <v>0</v>
+        <v>9</v>
+      </c>
+      <c r="D97" t="n">
+        <v>2.112676056338028</v>
       </c>
     </row>
     <row r="98">
@@ -1710,6 +2003,9 @@
       <c r="C98" t="n">
         <v>0</v>
       </c>
+      <c r="D98" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -1721,7 +2017,10 @@
         <v>149</v>
       </c>
       <c r="C99" t="n">
-        <v>0</v>
+        <v>27</v>
+      </c>
+      <c r="D99" t="n">
+        <v>6.04026845637584</v>
       </c>
     </row>
     <row r="100">
@@ -1736,6 +2035,9 @@
       <c r="C100" t="n">
         <v>0</v>
       </c>
+      <c r="D100" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -1749,6 +2051,9 @@
       <c r="C101" t="n">
         <v>0</v>
       </c>
+      <c r="D101" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -1760,7 +2065,10 @@
         <v>30</v>
       </c>
       <c r="C102" t="n">
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="D102" t="n">
+        <v>6.666666666666667</v>
       </c>
     </row>
     <row r="103">
@@ -1773,7 +2081,10 @@
         <v>42</v>
       </c>
       <c r="C103" t="n">
-        <v>0</v>
+        <v>15</v>
+      </c>
+      <c r="D103" t="n">
+        <v>11.9047619047619</v>
       </c>
     </row>
     <row r="104">
@@ -1788,6 +2099,9 @@
       <c r="C104" t="n">
         <v>0</v>
       </c>
+      <c r="D104" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -1799,7 +2113,10 @@
         <v>61</v>
       </c>
       <c r="C105" t="n">
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="D105" t="n">
+        <v>3.278688524590164</v>
       </c>
     </row>
     <row r="106">
@@ -1814,6 +2131,9 @@
       <c r="C106" t="n">
         <v>0</v>
       </c>
+      <c r="D106" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -1825,7 +2145,10 @@
         <v>92</v>
       </c>
       <c r="C107" t="n">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="D107" t="n">
+        <v>1.08695652173913</v>
       </c>
     </row>
     <row r="108">
@@ -1840,6 +2163,9 @@
       <c r="C108" t="n">
         <v>0</v>
       </c>
+      <c r="D108" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
@@ -1851,7 +2177,10 @@
         <v>61</v>
       </c>
       <c r="C109" t="n">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="D109" t="n">
+        <v>1.639344262295082</v>
       </c>
     </row>
     <row r="110">
@@ -1866,6 +2195,9 @@
       <c r="C110" t="n">
         <v>0</v>
       </c>
+      <c r="D110" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
@@ -1877,7 +2209,10 @@
         <v>60</v>
       </c>
       <c r="C111" t="n">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="D111" t="n">
+        <v>1.666666666666667</v>
       </c>
     </row>
     <row r="112">
@@ -1892,6 +2227,9 @@
       <c r="C112" t="n">
         <v>0</v>
       </c>
+      <c r="D112" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
@@ -1905,6 +2243,9 @@
       <c r="C113" t="n">
         <v>0</v>
       </c>
+      <c r="D113" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
@@ -1918,6 +2259,9 @@
       <c r="C114" t="n">
         <v>0</v>
       </c>
+      <c r="D114" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
@@ -1929,7 +2273,10 @@
         <v>60</v>
       </c>
       <c r="C115" t="n">
-        <v>0</v>
+        <v>9</v>
+      </c>
+      <c r="D115" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="116">
@@ -1944,6 +2291,9 @@
       <c r="C116" t="n">
         <v>0</v>
       </c>
+      <c r="D116" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
@@ -1955,7 +2305,10 @@
         <v>74</v>
       </c>
       <c r="C117" t="n">
-        <v>0</v>
+        <v>9</v>
+      </c>
+      <c r="D117" t="n">
+        <v>4.054054054054054</v>
       </c>
     </row>
     <row r="118">
@@ -1970,6 +2323,9 @@
       <c r="C118" t="n">
         <v>0</v>
       </c>
+      <c r="D118" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
@@ -1981,7 +2337,10 @@
         <v>60</v>
       </c>
       <c r="C119" t="n">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="D119" t="n">
+        <v>1.666666666666667</v>
       </c>
     </row>
     <row r="120">
@@ -1996,6 +2355,9 @@
       <c r="C120" t="n">
         <v>0</v>
       </c>
+      <c r="D120" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
@@ -2009,6 +2371,9 @@
       <c r="C121" t="n">
         <v>0</v>
       </c>
+      <c r="D121" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
@@ -2022,6 +2387,9 @@
       <c r="C122" t="n">
         <v>0</v>
       </c>
+      <c r="D122" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
@@ -2033,7 +2401,10 @@
         <v>60</v>
       </c>
       <c r="C123" t="n">
-        <v>0</v>
+        <v>9</v>
+      </c>
+      <c r="D123" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="124">
@@ -2048,6 +2419,9 @@
       <c r="C124" t="n">
         <v>0</v>
       </c>
+      <c r="D124" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
@@ -2059,7 +2433,10 @@
         <v>60</v>
       </c>
       <c r="C125" t="n">
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="D125" t="n">
+        <v>3.333333333333333</v>
       </c>
     </row>
     <row r="126">
@@ -2074,6 +2451,9 @@
       <c r="C126" t="n">
         <v>0</v>
       </c>
+      <c r="D126" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
@@ -2085,7 +2465,10 @@
         <v>60</v>
       </c>
       <c r="C127" t="n">
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="D127" t="n">
+        <v>3.333333333333333</v>
       </c>
     </row>
     <row r="128">
@@ -2100,6 +2483,9 @@
       <c r="C128" t="n">
         <v>0</v>
       </c>
+      <c r="D128" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
@@ -2113,6 +2499,9 @@
       <c r="C129" t="n">
         <v>0</v>
       </c>
+      <c r="D129" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
@@ -2126,6 +2515,9 @@
       <c r="C130" t="n">
         <v>0</v>
       </c>
+      <c r="D130" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
@@ -2139,6 +2531,9 @@
       <c r="C131" t="n">
         <v>0</v>
       </c>
+      <c r="D131" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
@@ -2150,7 +2545,10 @@
         <v>30</v>
       </c>
       <c r="C132" t="n">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="D132" t="n">
+        <v>3.333333333333333</v>
       </c>
     </row>
     <row r="133">
@@ -2165,6 +2563,9 @@
       <c r="C133" t="n">
         <v>0</v>
       </c>
+      <c r="D133" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
@@ -2178,6 +2579,9 @@
       <c r="C134" t="n">
         <v>0</v>
       </c>
+      <c r="D134" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
@@ -2191,6 +2595,9 @@
       <c r="C135" t="n">
         <v>0</v>
       </c>
+      <c r="D135" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
@@ -2204,6 +2611,9 @@
       <c r="C136" t="n">
         <v>0</v>
       </c>
+      <c r="D136" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
@@ -2217,6 +2627,9 @@
       <c r="C137" t="n">
         <v>0</v>
       </c>
+      <c r="D137" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
@@ -2230,6 +2643,9 @@
       <c r="C138" t="n">
         <v>0</v>
       </c>
+      <c r="D138" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
@@ -2243,6 +2659,9 @@
       <c r="C139" t="n">
         <v>0</v>
       </c>
+      <c r="D139" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
@@ -2256,6 +2675,9 @@
       <c r="C140" t="n">
         <v>0</v>
       </c>
+      <c r="D140" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
@@ -2269,6 +2691,9 @@
       <c r="C141" t="n">
         <v>0</v>
       </c>
+      <c r="D141" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
@@ -2280,7 +2705,10 @@
         <v>40</v>
       </c>
       <c r="C142" t="n">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="D142" t="n">
+        <v>2.5</v>
       </c>
     </row>
     <row r="143">
@@ -2295,6 +2723,9 @@
       <c r="C143" t="n">
         <v>0</v>
       </c>
+      <c r="D143" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
@@ -2308,6 +2739,9 @@
       <c r="C144" t="n">
         <v>0</v>
       </c>
+      <c r="D144" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
@@ -2319,7 +2753,10 @@
         <v>60</v>
       </c>
       <c r="C145" t="n">
-        <v>0</v>
+        <v>12</v>
+      </c>
+      <c r="D145" t="n">
+        <v>6.666666666666667</v>
       </c>
     </row>
     <row r="146">
@@ -2332,7 +2769,10 @@
         <v>75</v>
       </c>
       <c r="C146" t="n">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="D146" t="n">
+        <v>1.333333333333333</v>
       </c>
     </row>
     <row r="147">
@@ -2347,6 +2787,9 @@
       <c r="C147" t="n">
         <v>0</v>
       </c>
+      <c r="D147" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
@@ -2360,6 +2803,9 @@
       <c r="C148" t="n">
         <v>0</v>
       </c>
+      <c r="D148" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
@@ -2371,7 +2817,10 @@
         <v>61</v>
       </c>
       <c r="C149" t="n">
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="D149" t="n">
+        <v>3.278688524590164</v>
       </c>
     </row>
     <row r="150">
@@ -2386,6 +2835,9 @@
       <c r="C150" t="n">
         <v>0</v>
       </c>
+      <c r="D150" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
@@ -2399,6 +2851,9 @@
       <c r="C151" t="n">
         <v>0</v>
       </c>
+      <c r="D151" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
@@ -2412,6 +2867,9 @@
       <c r="C152" t="n">
         <v>0</v>
       </c>
+      <c r="D152" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
@@ -2423,7 +2881,10 @@
         <v>72</v>
       </c>
       <c r="C153" t="n">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="D153" t="n">
+        <v>1.388888888888889</v>
       </c>
     </row>
     <row r="154">
@@ -2438,6 +2899,9 @@
       <c r="C154" t="n">
         <v>0</v>
       </c>
+      <c r="D154" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
@@ -2449,7 +2913,10 @@
         <v>70</v>
       </c>
       <c r="C155" t="n">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="D155" t="n">
+        <v>1.428571428571429</v>
       </c>
     </row>
     <row r="156">
@@ -2464,6 +2931,9 @@
       <c r="C156" t="n">
         <v>0</v>
       </c>
+      <c r="D156" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
@@ -2475,7 +2945,10 @@
         <v>55</v>
       </c>
       <c r="C157" t="n">
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="D157" t="n">
+        <v>3.636363636363636</v>
       </c>
     </row>
     <row r="158">
@@ -2488,7 +2961,10 @@
         <v>97</v>
       </c>
       <c r="C158" t="n">
-        <v>0</v>
+        <v>9</v>
+      </c>
+      <c r="D158" t="n">
+        <v>3.092783505154639</v>
       </c>
     </row>
     <row r="159">
@@ -2501,7 +2977,10 @@
         <v>44</v>
       </c>
       <c r="C159" t="n">
-        <v>0</v>
+        <v>12</v>
+      </c>
+      <c r="D159" t="n">
+        <v>9.090909090909092</v>
       </c>
     </row>
     <row r="160">
@@ -2516,6 +2995,9 @@
       <c r="C160" t="n">
         <v>0</v>
       </c>
+      <c r="D160" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
@@ -2529,6 +3011,9 @@
       <c r="C161" t="n">
         <v>0</v>
       </c>
+      <c r="D161" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
@@ -2540,7 +3025,10 @@
         <v>40</v>
       </c>
       <c r="C162" t="n">
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="D162" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="163">
@@ -2555,6 +3043,9 @@
       <c r="C163" t="n">
         <v>0</v>
       </c>
+      <c r="D163" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
@@ -2568,6 +3059,9 @@
       <c r="C164" t="n">
         <v>0</v>
       </c>
+      <c r="D164" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
@@ -2579,7 +3073,10 @@
         <v>76</v>
       </c>
       <c r="C165" t="n">
-        <v>0</v>
+        <v>12</v>
+      </c>
+      <c r="D165" t="n">
+        <v>5.263157894736842</v>
       </c>
     </row>
     <row r="166">
@@ -2594,6 +3091,9 @@
       <c r="C166" t="n">
         <v>0</v>
       </c>
+      <c r="D166" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
@@ -2607,6 +3107,9 @@
       <c r="C167" t="n">
         <v>0</v>
       </c>
+      <c r="D167" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
@@ -2620,6 +3123,9 @@
       <c r="C168" t="n">
         <v>0</v>
       </c>
+      <c r="D168" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
@@ -2633,6 +3139,9 @@
       <c r="C169" t="n">
         <v>0</v>
       </c>
+      <c r="D169" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
@@ -2646,6 +3155,9 @@
       <c r="C170" t="n">
         <v>0</v>
       </c>
+      <c r="D170" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
@@ -2657,7 +3169,10 @@
         <v>30</v>
       </c>
       <c r="C171" t="n">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="D171" t="n">
+        <v>3.333333333333333</v>
       </c>
     </row>
     <row r="172">
@@ -2670,7 +3185,10 @@
         <v>77</v>
       </c>
       <c r="C172" t="n">
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="D172" t="n">
+        <v>2.597402597402597</v>
       </c>
     </row>
     <row r="173">
@@ -2683,7 +3201,10 @@
         <v>30</v>
       </c>
       <c r="C173" t="n">
-        <v>0</v>
+        <v>9</v>
+      </c>
+      <c r="D173" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="174">
@@ -2696,7 +3217,10 @@
         <v>30</v>
       </c>
       <c r="C174" t="n">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="D174" t="n">
+        <v>3.333333333333333</v>
       </c>
     </row>
     <row r="175">
@@ -2709,7 +3233,10 @@
         <v>57</v>
       </c>
       <c r="C175" t="n">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="D175" t="n">
+        <v>1.754385964912281</v>
       </c>
     </row>
     <row r="176">
@@ -2724,6 +3251,9 @@
       <c r="C176" t="n">
         <v>0</v>
       </c>
+      <c r="D176" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
@@ -2737,6 +3267,9 @@
       <c r="C177" t="n">
         <v>0</v>
       </c>
+      <c r="D177" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
@@ -2750,6 +3283,9 @@
       <c r="C178" t="n">
         <v>0</v>
       </c>
+      <c r="D178" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
@@ -2763,6 +3299,9 @@
       <c r="C179" t="n">
         <v>0</v>
       </c>
+      <c r="D179" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
@@ -2776,6 +3315,9 @@
       <c r="C180" t="n">
         <v>0</v>
       </c>
+      <c r="D180" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
@@ -2789,6 +3331,9 @@
       <c r="C181" t="n">
         <v>0</v>
       </c>
+      <c r="D181" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
@@ -2800,7 +3345,10 @@
         <v>71</v>
       </c>
       <c r="C182" t="n">
-        <v>0</v>
+        <v>12</v>
+      </c>
+      <c r="D182" t="n">
+        <v>5.633802816901409</v>
       </c>
     </row>
     <row r="183">
@@ -2813,7 +3361,10 @@
         <v>60</v>
       </c>
       <c r="C183" t="n">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="D183" t="n">
+        <v>1.666666666666667</v>
       </c>
     </row>
     <row r="184">
@@ -2826,7 +3377,10 @@
         <v>346</v>
       </c>
       <c r="C184" t="n">
-        <v>0</v>
+        <v>45</v>
+      </c>
+      <c r="D184" t="n">
+        <v>4.335260115606936</v>
       </c>
     </row>
     <row r="185">
@@ -2839,7 +3393,10 @@
         <v>271</v>
       </c>
       <c r="C185" t="n">
-        <v>0</v>
+        <v>39</v>
+      </c>
+      <c r="D185" t="n">
+        <v>4.797047970479705</v>
       </c>
     </row>
     <row r="186">
@@ -2852,7 +3409,10 @@
         <v>139</v>
       </c>
       <c r="C186" t="n">
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="D186" t="n">
+        <v>1.43884892086331</v>
       </c>
     </row>
     <row r="187">
@@ -2865,7 +3425,10 @@
         <v>125</v>
       </c>
       <c r="C187" t="n">
-        <v>0</v>
+        <v>9</v>
+      </c>
+      <c r="D187" t="n">
+        <v>2.4</v>
       </c>
     </row>
     <row r="188">
@@ -2878,7 +3441,10 @@
         <v>136</v>
       </c>
       <c r="C188" t="n">
-        <v>0</v>
+        <v>9</v>
+      </c>
+      <c r="D188" t="n">
+        <v>2.205882352941177</v>
       </c>
     </row>
     <row r="189">
@@ -2891,7 +3457,10 @@
         <v>184</v>
       </c>
       <c r="C189" t="n">
-        <v>0</v>
+        <v>21</v>
+      </c>
+      <c r="D189" t="n">
+        <v>3.804347826086957</v>
       </c>
     </row>
     <row r="190">
@@ -2906,6 +3475,9 @@
       <c r="C190" t="n">
         <v>0</v>
       </c>
+      <c r="D190" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
@@ -2919,6 +3491,9 @@
       <c r="C191" t="n">
         <v>0</v>
       </c>
+      <c r="D191" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
@@ -2930,7 +3505,10 @@
         <v>85</v>
       </c>
       <c r="C192" t="n">
-        <v>0</v>
+        <v>18</v>
+      </c>
+      <c r="D192" t="n">
+        <v>7.058823529411764</v>
       </c>
     </row>
     <row r="193">
@@ -2943,7 +3521,10 @@
         <v>110</v>
       </c>
       <c r="C193" t="n">
-        <v>0</v>
+        <v>15</v>
+      </c>
+      <c r="D193" t="n">
+        <v>4.545454545454546</v>
       </c>
     </row>
     <row r="194">
@@ -2956,7 +3537,10 @@
         <v>77</v>
       </c>
       <c r="C194" t="n">
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="D194" t="n">
+        <v>2.597402597402597</v>
       </c>
     </row>
     <row r="195">
@@ -2971,6 +3555,9 @@
       <c r="C195" t="n">
         <v>0</v>
       </c>
+      <c r="D195" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
@@ -2982,7 +3569,10 @@
         <v>36</v>
       </c>
       <c r="C196" t="n">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="D196" t="n">
+        <v>2.777777777777778</v>
       </c>
     </row>
     <row r="197">
@@ -2995,7 +3585,10 @@
         <v>57</v>
       </c>
       <c r="C197" t="n">
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="D197" t="n">
+        <v>3.508771929824561</v>
       </c>
     </row>
     <row r="198">
@@ -3010,6 +3603,9 @@
       <c r="C198" t="n">
         <v>0</v>
       </c>
+      <c r="D198" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="199">
       <c r="A199" t="inlineStr">
@@ -3021,7 +3617,10 @@
         <v>92</v>
       </c>
       <c r="C199" t="n">
-        <v>0</v>
+        <v>9</v>
+      </c>
+      <c r="D199" t="n">
+        <v>3.260869565217391</v>
       </c>
     </row>
     <row r="200">
@@ -3036,6 +3635,9 @@
       <c r="C200" t="n">
         <v>0</v>
       </c>
+      <c r="D200" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="201">
       <c r="A201" t="inlineStr">
@@ -3049,6 +3651,9 @@
       <c r="C201" t="n">
         <v>0</v>
       </c>
+      <c r="D201" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="202">
       <c r="A202" t="inlineStr">
@@ -3062,6 +3667,9 @@
       <c r="C202" t="n">
         <v>0</v>
       </c>
+      <c r="D202" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="203">
       <c r="A203" t="inlineStr">
@@ -3075,6 +3683,9 @@
       <c r="C203" t="n">
         <v>0</v>
       </c>
+      <c r="D203" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="204">
       <c r="A204" t="inlineStr">
@@ -3086,7 +3697,10 @@
         <v>115</v>
       </c>
       <c r="C204" t="n">
-        <v>0</v>
+        <v>9</v>
+      </c>
+      <c r="D204" t="n">
+        <v>2.608695652173913</v>
       </c>
     </row>
     <row r="205">
@@ -3099,7 +3713,10 @@
         <v>124</v>
       </c>
       <c r="C205" t="n">
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="D205" t="n">
+        <v>1.612903225806452</v>
       </c>
     </row>
     <row r="206">
@@ -3112,7 +3729,10 @@
         <v>129</v>
       </c>
       <c r="C206" t="n">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="D206" t="n">
+        <v>0.7751937984496124</v>
       </c>
     </row>
     <row r="207">
@@ -3125,7 +3745,10 @@
         <v>65</v>
       </c>
       <c r="C207" t="n">
-        <v>0</v>
+        <v>9</v>
+      </c>
+      <c r="D207" t="n">
+        <v>4.615384615384616</v>
       </c>
     </row>
     <row r="208">
@@ -3138,7 +3761,10 @@
         <v>124</v>
       </c>
       <c r="C208" t="n">
-        <v>0</v>
+        <v>12</v>
+      </c>
+      <c r="D208" t="n">
+        <v>3.225806451612903</v>
       </c>
     </row>
     <row r="209">
@@ -3151,7 +3777,10 @@
         <v>67</v>
       </c>
       <c r="C209" t="n">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="D209" t="n">
+        <v>1.492537313432836</v>
       </c>
     </row>
     <row r="210">
@@ -3164,7 +3793,10 @@
         <v>104</v>
       </c>
       <c r="C210" t="n">
-        <v>0</v>
+        <v>21</v>
+      </c>
+      <c r="D210" t="n">
+        <v>6.730769230769231</v>
       </c>
     </row>
     <row r="211">
@@ -3177,7 +3809,10 @@
         <v>81</v>
       </c>
       <c r="C211" t="n">
-        <v>0</v>
+        <v>18</v>
+      </c>
+      <c r="D211" t="n">
+        <v>7.407407407407407</v>
       </c>
     </row>
     <row r="212">
@@ -3190,7 +3825,10 @@
         <v>145</v>
       </c>
       <c r="C212" t="n">
-        <v>0</v>
+        <v>15</v>
+      </c>
+      <c r="D212" t="n">
+        <v>3.448275862068965</v>
       </c>
     </row>
     <row r="213">
@@ -3203,7 +3841,10 @@
         <v>128</v>
       </c>
       <c r="C213" t="n">
-        <v>0</v>
+        <v>21</v>
+      </c>
+      <c r="D213" t="n">
+        <v>5.46875</v>
       </c>
     </row>
     <row r="214">
@@ -3216,7 +3857,10 @@
         <v>216</v>
       </c>
       <c r="C214" t="n">
-        <v>0</v>
+        <v>30</v>
+      </c>
+      <c r="D214" t="n">
+        <v>4.62962962962963</v>
       </c>
     </row>
     <row r="215">
@@ -3229,7 +3873,10 @@
         <v>157</v>
       </c>
       <c r="C215" t="n">
-        <v>0</v>
+        <v>42</v>
+      </c>
+      <c r="D215" t="n">
+        <v>8.917197452229299</v>
       </c>
     </row>
     <row r="216">
@@ -3242,7 +3889,10 @@
         <v>325</v>
       </c>
       <c r="C216" t="n">
-        <v>0</v>
+        <v>33</v>
+      </c>
+      <c r="D216" t="n">
+        <v>3.384615384615385</v>
       </c>
     </row>
     <row r="217">
@@ -3255,7 +3905,10 @@
         <v>318</v>
       </c>
       <c r="C217" t="n">
-        <v>0</v>
+        <v>15</v>
+      </c>
+      <c r="D217" t="n">
+        <v>1.572327044025157</v>
       </c>
     </row>
     <row r="218">
@@ -3270,6 +3923,9 @@
       <c r="C218" t="n">
         <v>0</v>
       </c>
+      <c r="D218" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="219">
       <c r="A219" t="inlineStr">
@@ -3281,7 +3937,10 @@
         <v>223</v>
       </c>
       <c r="C219" t="n">
-        <v>0</v>
+        <v>57</v>
+      </c>
+      <c r="D219" t="n">
+        <v>8.520179372197308</v>
       </c>
     </row>
     <row r="220">
@@ -3294,7 +3953,10 @@
         <v>162</v>
       </c>
       <c r="C220" t="n">
-        <v>0</v>
+        <v>45</v>
+      </c>
+      <c r="D220" t="n">
+        <v>9.25925925925926</v>
       </c>
     </row>
     <row r="221">
@@ -3307,7 +3969,10 @@
         <v>217</v>
       </c>
       <c r="C221" t="n">
-        <v>0</v>
+        <v>51</v>
+      </c>
+      <c r="D221" t="n">
+        <v>7.834101382488479</v>
       </c>
     </row>
     <row r="222">
@@ -3320,7 +3985,10 @@
         <v>190</v>
       </c>
       <c r="C222" t="n">
-        <v>0</v>
+        <v>15</v>
+      </c>
+      <c r="D222" t="n">
+        <v>2.631578947368421</v>
       </c>
     </row>
     <row r="223">
@@ -3333,7 +4001,10 @@
         <v>181</v>
       </c>
       <c r="C223" t="n">
-        <v>0</v>
+        <v>24</v>
+      </c>
+      <c r="D223" t="n">
+        <v>4.41988950276243</v>
       </c>
     </row>
     <row r="224">
@@ -3346,7 +4017,10 @@
         <v>183</v>
       </c>
       <c r="C224" t="n">
-        <v>0</v>
+        <v>21</v>
+      </c>
+      <c r="D224" t="n">
+        <v>3.825136612021858</v>
       </c>
     </row>
     <row r="225">
@@ -3359,7 +4033,10 @@
         <v>267</v>
       </c>
       <c r="C225" t="n">
-        <v>0</v>
+        <v>27</v>
+      </c>
+      <c r="D225" t="n">
+        <v>3.370786516853932</v>
       </c>
     </row>
     <row r="226">
@@ -3372,7 +4049,10 @@
         <v>224</v>
       </c>
       <c r="C226" t="n">
-        <v>0</v>
+        <v>18</v>
+      </c>
+      <c r="D226" t="n">
+        <v>2.678571428571428</v>
       </c>
     </row>
     <row r="227">
@@ -3385,7 +4065,10 @@
         <v>363</v>
       </c>
       <c r="C227" t="n">
-        <v>0</v>
+        <v>27</v>
+      </c>
+      <c r="D227" t="n">
+        <v>2.479338842975207</v>
       </c>
     </row>
     <row r="228">
@@ -3398,7 +4081,10 @@
         <v>283</v>
       </c>
       <c r="C228" t="n">
-        <v>0</v>
+        <v>18</v>
+      </c>
+      <c r="D228" t="n">
+        <v>2.120141342756184</v>
       </c>
     </row>
     <row r="229">
@@ -3411,7 +4097,10 @@
         <v>256</v>
       </c>
       <c r="C229" t="n">
-        <v>0</v>
+        <v>39</v>
+      </c>
+      <c r="D229" t="n">
+        <v>5.078125</v>
       </c>
     </row>
     <row r="230">
@@ -3424,7 +4113,10 @@
         <v>232</v>
       </c>
       <c r="C230" t="n">
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="D230" t="n">
+        <v>0.8620689655172413</v>
       </c>
     </row>
     <row r="231">
@@ -3437,7 +4129,10 @@
         <v>473</v>
       </c>
       <c r="C231" t="n">
-        <v>0</v>
+        <v>18</v>
+      </c>
+      <c r="D231" t="n">
+        <v>1.268498942917548</v>
       </c>
     </row>
     <row r="232">
@@ -3450,7 +4145,10 @@
         <v>273</v>
       </c>
       <c r="C232" t="n">
-        <v>0</v>
+        <v>12</v>
+      </c>
+      <c r="D232" t="n">
+        <v>1.465201465201465</v>
       </c>
     </row>
     <row r="233">
@@ -3465,6 +4163,9 @@
       <c r="C233" t="n">
         <v>0</v>
       </c>
+      <c r="D233" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="234">
       <c r="A234" t="inlineStr">
@@ -3476,7 +4177,10 @@
         <v>184</v>
       </c>
       <c r="C234" t="n">
-        <v>0</v>
+        <v>36</v>
+      </c>
+      <c r="D234" t="n">
+        <v>6.521739130434782</v>
       </c>
     </row>
     <row r="235">
@@ -3491,6 +4195,9 @@
       <c r="C235" t="n">
         <v>0</v>
       </c>
+      <c r="D235" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="236">
       <c r="A236" t="inlineStr">
@@ -3502,7 +4209,10 @@
         <v>127</v>
       </c>
       <c r="C236" t="n">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="D236" t="n">
+        <v>0.7874015748031495</v>
       </c>
     </row>
     <row r="237">
@@ -3515,7 +4225,10 @@
         <v>113</v>
       </c>
       <c r="C237" t="n">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="D237" t="n">
+        <v>0.8849557522123894</v>
       </c>
     </row>
     <row r="238">
@@ -3530,6 +4243,9 @@
       <c r="C238" t="n">
         <v>0</v>
       </c>
+      <c r="D238" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="239">
       <c r="A239" t="inlineStr">
@@ -3543,6 +4259,9 @@
       <c r="C239" t="n">
         <v>0</v>
       </c>
+      <c r="D239" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="240">
       <c r="A240" t="inlineStr">
@@ -3556,6 +4275,9 @@
       <c r="C240" t="n">
         <v>0</v>
       </c>
+      <c r="D240" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="241">
       <c r="A241" t="inlineStr">
@@ -3567,7 +4289,10 @@
         <v>145</v>
       </c>
       <c r="C241" t="n">
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="D241" t="n">
+        <v>1.379310344827586</v>
       </c>
     </row>
     <row r="242">
@@ -3580,7 +4305,10 @@
         <v>184</v>
       </c>
       <c r="C242" t="n">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="D242" t="n">
+        <v>0.5434782608695652</v>
       </c>
     </row>
     <row r="243">
@@ -3593,7 +4321,10 @@
         <v>110</v>
       </c>
       <c r="C243" t="n">
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="D243" t="n">
+        <v>1.818181818181818</v>
       </c>
     </row>
     <row r="244">
@@ -3606,7 +4337,10 @@
         <v>253</v>
       </c>
       <c r="C244" t="n">
-        <v>0</v>
+        <v>21</v>
+      </c>
+      <c r="D244" t="n">
+        <v>2.766798418972332</v>
       </c>
     </row>
     <row r="245">
@@ -3621,6 +4355,9 @@
       <c r="C245" t="n">
         <v>0</v>
       </c>
+      <c r="D245" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="246">
       <c r="A246" t="inlineStr">
@@ -3632,7 +4369,10 @@
         <v>143</v>
       </c>
       <c r="C246" t="n">
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="D246" t="n">
+        <v>1.398601398601399</v>
       </c>
     </row>
     <row r="247">
@@ -3645,7 +4385,10 @@
         <v>55</v>
       </c>
       <c r="C247" t="n">
-        <v>0</v>
+        <v>9</v>
+      </c>
+      <c r="D247" t="n">
+        <v>5.454545454545454</v>
       </c>
     </row>
     <row r="248">
@@ -3658,7 +4401,10 @@
         <v>60</v>
       </c>
       <c r="C248" t="n">
-        <v>0</v>
+        <v>9</v>
+      </c>
+      <c r="D248" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="249">
@@ -3671,7 +4417,10 @@
         <v>160</v>
       </c>
       <c r="C249" t="n">
-        <v>0</v>
+        <v>12</v>
+      </c>
+      <c r="D249" t="n">
+        <v>2.5</v>
       </c>
     </row>
     <row r="250">
@@ -3686,6 +4435,9 @@
       <c r="C250" t="n">
         <v>0</v>
       </c>
+      <c r="D250" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="251">
       <c r="A251" t="inlineStr">
@@ -3697,7 +4449,10 @@
         <v>95</v>
       </c>
       <c r="C251" t="n">
-        <v>0</v>
+        <v>9</v>
+      </c>
+      <c r="D251" t="n">
+        <v>3.157894736842105</v>
       </c>
     </row>
     <row r="252">
@@ -3710,7 +4465,10 @@
         <v>40</v>
       </c>
       <c r="C252" t="n">
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="D252" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="253">
@@ -3725,6 +4483,9 @@
       <c r="C253" t="n">
         <v>0</v>
       </c>
+      <c r="D253" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="254">
       <c r="A254" t="inlineStr">
@@ -3736,7 +4497,10 @@
         <v>160</v>
       </c>
       <c r="C254" t="n">
-        <v>0</v>
+        <v>9</v>
+      </c>
+      <c r="D254" t="n">
+        <v>1.875</v>
       </c>
     </row>
     <row r="255">
@@ -3749,7 +4513,10 @@
         <v>40</v>
       </c>
       <c r="C255" t="n">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="D255" t="n">
+        <v>2.5</v>
       </c>
     </row>
     <row r="256">
@@ -3762,7 +4529,10 @@
         <v>145</v>
       </c>
       <c r="C256" t="n">
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="D256" t="n">
+        <v>1.379310344827586</v>
       </c>
     </row>
     <row r="257">
@@ -3775,7 +4545,10 @@
         <v>233</v>
       </c>
       <c r="C257" t="n">
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="D257" t="n">
+        <v>0.8583690987124464</v>
       </c>
     </row>
     <row r="258">
@@ -3788,7 +4561,10 @@
         <v>80</v>
       </c>
       <c r="C258" t="n">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="D258" t="n">
+        <v>1.25</v>
       </c>
     </row>
     <row r="259">
@@ -3801,7 +4577,10 @@
         <v>110</v>
       </c>
       <c r="C259" t="n">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="D259" t="n">
+        <v>0.9090909090909091</v>
       </c>
     </row>
     <row r="260">
@@ -3814,7 +4593,10 @@
         <v>120</v>
       </c>
       <c r="C260" t="n">
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="D260" t="n">
+        <v>1.666666666666667</v>
       </c>
     </row>
     <row r="261">
@@ -3829,6 +4611,9 @@
       <c r="C261" t="n">
         <v>0</v>
       </c>
+      <c r="D261" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="262">
       <c r="A262" t="inlineStr">
@@ -3840,7 +4625,10 @@
         <v>120</v>
       </c>
       <c r="C262" t="n">
-        <v>0</v>
+        <v>9</v>
+      </c>
+      <c r="D262" t="n">
+        <v>2.5</v>
       </c>
     </row>
     <row r="263">
@@ -3855,6 +4643,9 @@
       <c r="C263" t="n">
         <v>0</v>
       </c>
+      <c r="D263" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="264">
       <c r="A264" t="inlineStr">
@@ -3866,7 +4657,10 @@
         <v>91</v>
       </c>
       <c r="C264" t="n">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="D264" t="n">
+        <v>1.098901098901099</v>
       </c>
     </row>
     <row r="265">
@@ -3879,7 +4673,10 @@
         <v>233</v>
       </c>
       <c r="C265" t="n">
-        <v>0</v>
+        <v>27</v>
+      </c>
+      <c r="D265" t="n">
+        <v>3.862660944206009</v>
       </c>
     </row>
     <row r="266">
@@ -3892,7 +4689,10 @@
         <v>105</v>
       </c>
       <c r="C266" t="n">
-        <v>0</v>
+        <v>27</v>
+      </c>
+      <c r="D266" t="n">
+        <v>8.571428571428571</v>
       </c>
     </row>
     <row r="267">
@@ -3905,7 +4705,10 @@
         <v>57</v>
       </c>
       <c r="C267" t="n">
-        <v>0</v>
+        <v>15</v>
+      </c>
+      <c r="D267" t="n">
+        <v>8.771929824561402</v>
       </c>
     </row>
     <row r="268">
@@ -3918,7 +4721,10 @@
         <v>30</v>
       </c>
       <c r="C268" t="n">
-        <v>0</v>
+        <v>9</v>
+      </c>
+      <c r="D268" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="269">
@@ -3933,6 +4739,9 @@
       <c r="C269" t="n">
         <v>0</v>
       </c>
+      <c r="D269" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="270">
       <c r="A270" t="inlineStr">
@@ -3944,7 +4753,10 @@
         <v>40</v>
       </c>
       <c r="C270" t="n">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="D270" t="n">
+        <v>2.5</v>
       </c>
     </row>
     <row r="271">
@@ -3957,7 +4769,10 @@
         <v>110</v>
       </c>
       <c r="C271" t="n">
-        <v>0</v>
+        <v>15</v>
+      </c>
+      <c r="D271" t="n">
+        <v>4.545454545454546</v>
       </c>
     </row>
     <row r="272">
@@ -3970,7 +4785,10 @@
         <v>40</v>
       </c>
       <c r="C272" t="n">
-        <v>0</v>
+        <v>24</v>
+      </c>
+      <c r="D272" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="273">
@@ -3983,7 +4801,10 @@
         <v>40</v>
       </c>
       <c r="C273" t="n">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="D273" t="n">
+        <v>2.5</v>
       </c>
     </row>
     <row r="274">
@@ -3998,6 +4819,9 @@
       <c r="C274" t="n">
         <v>0</v>
       </c>
+      <c r="D274" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="275">
       <c r="A275" t="inlineStr">
@@ -4011,6 +4835,9 @@
       <c r="C275" t="n">
         <v>0</v>
       </c>
+      <c r="D275" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="276">
       <c r="A276" t="inlineStr">
@@ -4024,6 +4851,9 @@
       <c r="C276" t="n">
         <v>0</v>
       </c>
+      <c r="D276" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="277">
       <c r="A277" t="inlineStr">
@@ -4035,7 +4865,10 @@
         <v>60</v>
       </c>
       <c r="C277" t="n">
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="D277" t="n">
+        <v>3.333333333333333</v>
       </c>
     </row>
     <row r="278">
@@ -4050,6 +4883,9 @@
       <c r="C278" t="n">
         <v>0</v>
       </c>
+      <c r="D278" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="279">
       <c r="A279" t="inlineStr">
@@ -4063,6 +4899,9 @@
       <c r="C279" t="n">
         <v>0</v>
       </c>
+      <c r="D279" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="280">
       <c r="A280" t="inlineStr">
@@ -4076,6 +4915,9 @@
       <c r="C280" t="n">
         <v>0</v>
       </c>
+      <c r="D280" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="281">
       <c r="A281" t="inlineStr">
@@ -4089,6 +4931,9 @@
       <c r="C281" t="n">
         <v>0</v>
       </c>
+      <c r="D281" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="282">
       <c r="A282" t="inlineStr">
@@ -4102,6 +4947,9 @@
       <c r="C282" t="n">
         <v>0</v>
       </c>
+      <c r="D282" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="283">
       <c r="A283" t="inlineStr">
@@ -4115,6 +4963,9 @@
       <c r="C283" t="n">
         <v>0</v>
       </c>
+      <c r="D283" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="284">
       <c r="A284" t="inlineStr">
@@ -4128,6 +4979,9 @@
       <c r="C284" t="n">
         <v>0</v>
       </c>
+      <c r="D284" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="285">
       <c r="A285" t="inlineStr">
@@ -4141,6 +4995,9 @@
       <c r="C285" t="n">
         <v>0</v>
       </c>
+      <c r="D285" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="286">
       <c r="A286" t="inlineStr">
@@ -4154,6 +5011,9 @@
       <c r="C286" t="n">
         <v>0</v>
       </c>
+      <c r="D286" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="287">
       <c r="A287" t="inlineStr">
@@ -4167,6 +5027,9 @@
       <c r="C287" t="n">
         <v>0</v>
       </c>
+      <c r="D287" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="288">
       <c r="A288" t="inlineStr">
@@ -4178,7 +5041,10 @@
         <v>32</v>
       </c>
       <c r="C288" t="n">
-        <v>0</v>
+        <v>15</v>
+      </c>
+      <c r="D288" t="n">
+        <v>15.625</v>
       </c>
     </row>
     <row r="289">
@@ -4193,6 +5059,9 @@
       <c r="C289" t="n">
         <v>0</v>
       </c>
+      <c r="D289" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="290">
       <c r="A290" t="inlineStr">
@@ -4206,6 +5075,9 @@
       <c r="C290" t="n">
         <v>0</v>
       </c>
+      <c r="D290" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="291">
       <c r="A291" t="inlineStr">
@@ -4217,7 +5089,10 @@
         <v>30</v>
       </c>
       <c r="C291" t="n">
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="D291" t="n">
+        <v>6.666666666666667</v>
       </c>
     </row>
     <row r="292">
@@ -4230,7 +5105,10 @@
         <v>30</v>
       </c>
       <c r="C292" t="n">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="D292" t="n">
+        <v>3.333333333333333</v>
       </c>
     </row>
     <row r="293">
@@ -4243,7 +5121,10 @@
         <v>70</v>
       </c>
       <c r="C293" t="n">
-        <v>0</v>
+        <v>15</v>
+      </c>
+      <c r="D293" t="n">
+        <v>7.142857142857142</v>
       </c>
     </row>
     <row r="294">
@@ -4256,7 +5137,10 @@
         <v>30</v>
       </c>
       <c r="C294" t="n">
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="D294" t="n">
+        <v>6.666666666666667</v>
       </c>
     </row>
     <row r="295">
@@ -4269,7 +5153,10 @@
         <v>30</v>
       </c>
       <c r="C295" t="n">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="D295" t="n">
+        <v>3.333333333333333</v>
       </c>
     </row>
     <row r="296">
@@ -4284,6 +5171,9 @@
       <c r="C296" t="n">
         <v>0</v>
       </c>
+      <c r="D296" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="297">
       <c r="A297" t="inlineStr">
@@ -4297,6 +5187,9 @@
       <c r="C297" t="n">
         <v>0</v>
       </c>
+      <c r="D297" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="298">
       <c r="A298" t="inlineStr">
@@ -4308,7 +5201,10 @@
         <v>40</v>
       </c>
       <c r="C298" t="n">
-        <v>0</v>
+        <v>15</v>
+      </c>
+      <c r="D298" t="n">
+        <v>12.5</v>
       </c>
     </row>
     <row r="299">
@@ -4321,7 +5217,10 @@
         <v>70</v>
       </c>
       <c r="C299" t="n">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="D299" t="n">
+        <v>1.428571428571429</v>
       </c>
     </row>
     <row r="300">
@@ -4334,7 +5233,10 @@
         <v>30</v>
       </c>
       <c r="C300" t="n">
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="D300" t="n">
+        <v>6.666666666666667</v>
       </c>
     </row>
     <row r="301">
@@ -4347,7 +5249,10 @@
         <v>60</v>
       </c>
       <c r="C301" t="n">
-        <v>0</v>
+        <v>12</v>
+      </c>
+      <c r="D301" t="n">
+        <v>6.666666666666667</v>
       </c>
     </row>
     <row r="302">
@@ -4360,7 +5265,10 @@
         <v>62</v>
       </c>
       <c r="C302" t="n">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="D302" t="n">
+        <v>1.612903225806452</v>
       </c>
     </row>
     <row r="303">
@@ -4375,6 +5283,9 @@
       <c r="C303" t="n">
         <v>0</v>
       </c>
+      <c r="D303" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="304">
       <c r="A304" t="inlineStr">
@@ -4388,6 +5299,9 @@
       <c r="C304" t="n">
         <v>0</v>
       </c>
+      <c r="D304" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="305">
       <c r="A305" t="inlineStr">
@@ -4401,6 +5315,9 @@
       <c r="C305" t="n">
         <v>0</v>
       </c>
+      <c r="D305" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="306">
       <c r="A306" t="inlineStr">
@@ -4412,7 +5329,10 @@
         <v>30</v>
       </c>
       <c r="C306" t="n">
-        <v>0</v>
+        <v>12</v>
+      </c>
+      <c r="D306" t="n">
+        <v>13.33333333333333</v>
       </c>
     </row>
     <row r="307">
@@ -4425,7 +5345,10 @@
         <v>40</v>
       </c>
       <c r="C307" t="n">
-        <v>0</v>
+        <v>12</v>
+      </c>
+      <c r="D307" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="308">
@@ -4438,7 +5361,10 @@
         <v>40</v>
       </c>
       <c r="C308" t="n">
-        <v>0</v>
+        <v>9</v>
+      </c>
+      <c r="D308" t="n">
+        <v>7.5</v>
       </c>
     </row>
     <row r="309">
@@ -4451,7 +5377,10 @@
         <v>30</v>
       </c>
       <c r="C309" t="n">
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="D309" t="n">
+        <v>6.666666666666667</v>
       </c>
     </row>
     <row r="310">
@@ -4466,6 +5395,9 @@
       <c r="C310" t="n">
         <v>0</v>
       </c>
+      <c r="D310" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="311">
       <c r="A311" t="inlineStr">
@@ -4477,7 +5409,10 @@
         <v>40</v>
       </c>
       <c r="C311" t="n">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="D311" t="n">
+        <v>2.5</v>
       </c>
     </row>
     <row r="312">
@@ -4490,7 +5425,10 @@
         <v>30</v>
       </c>
       <c r="C312" t="n">
-        <v>0</v>
+        <v>15</v>
+      </c>
+      <c r="D312" t="n">
+        <v>16.66666666666666</v>
       </c>
     </row>
     <row r="313">
@@ -4503,7 +5441,10 @@
         <v>30</v>
       </c>
       <c r="C313" t="n">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="D313" t="n">
+        <v>3.333333333333333</v>
       </c>
     </row>
     <row r="314">
@@ -4516,7 +5457,10 @@
         <v>30</v>
       </c>
       <c r="C314" t="n">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="D314" t="n">
+        <v>3.333333333333333</v>
       </c>
     </row>
     <row r="315">
@@ -4531,6 +5475,9 @@
       <c r="C315" t="n">
         <v>0</v>
       </c>
+      <c r="D315" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="316">
       <c r="A316" t="inlineStr">
@@ -4544,6 +5491,9 @@
       <c r="C316" t="n">
         <v>0</v>
       </c>
+      <c r="D316" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="317">
       <c r="A317" t="inlineStr">
@@ -4557,6 +5507,9 @@
       <c r="C317" t="n">
         <v>0</v>
       </c>
+      <c r="D317" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="318">
       <c r="A318" t="inlineStr">
@@ -4570,6 +5523,9 @@
       <c r="C318" t="n">
         <v>0</v>
       </c>
+      <c r="D318" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="319">
       <c r="A319" t="inlineStr">
@@ -4581,7 +5537,10 @@
         <v>30</v>
       </c>
       <c r="C319" t="n">
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="D319" t="n">
+        <v>6.666666666666667</v>
       </c>
     </row>
     <row r="320">
@@ -4596,6 +5555,9 @@
       <c r="C320" t="n">
         <v>0</v>
       </c>
+      <c r="D320" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="321">
       <c r="A321" t="inlineStr">
@@ -4609,6 +5571,9 @@
       <c r="C321" t="n">
         <v>0</v>
       </c>
+      <c r="D321" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="322">
       <c r="A322" t="inlineStr">
@@ -4620,7 +5585,10 @@
         <v>30</v>
       </c>
       <c r="C322" t="n">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="D322" t="n">
+        <v>3.333333333333333</v>
       </c>
     </row>
     <row r="323">
@@ -4635,6 +5603,9 @@
       <c r="C323" t="n">
         <v>0</v>
       </c>
+      <c r="D323" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="324">
       <c r="A324" t="inlineStr">
@@ -4648,6 +5619,9 @@
       <c r="C324" t="n">
         <v>0</v>
       </c>
+      <c r="D324" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="325">
       <c r="A325" t="inlineStr">
@@ -4661,6 +5635,9 @@
       <c r="C325" t="n">
         <v>0</v>
       </c>
+      <c r="D325" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="326">
       <c r="A326" t="inlineStr">
@@ -4674,6 +5651,9 @@
       <c r="C326" t="n">
         <v>0</v>
       </c>
+      <c r="D326" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="327">
       <c r="A327" t="inlineStr">
@@ -4685,7 +5665,10 @@
         <v>30</v>
       </c>
       <c r="C327" t="n">
-        <v>0</v>
+        <v>9</v>
+      </c>
+      <c r="D327" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="328">
@@ -4698,7 +5681,10 @@
         <v>35</v>
       </c>
       <c r="C328" t="n">
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="D328" t="n">
+        <v>5.714285714285714</v>
       </c>
     </row>
     <row r="329">
@@ -4711,7 +5697,10 @@
         <v>30</v>
       </c>
       <c r="C329" t="n">
-        <v>0</v>
+        <v>24</v>
+      </c>
+      <c r="D329" t="n">
+        <v>26.66666666666667</v>
       </c>
     </row>
     <row r="330">
@@ -4726,6 +5715,9 @@
       <c r="C330" t="n">
         <v>0</v>
       </c>
+      <c r="D330" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="331">
       <c r="A331" t="inlineStr">
@@ -4739,6 +5731,9 @@
       <c r="C331" t="n">
         <v>0</v>
       </c>
+      <c r="D331" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="332">
       <c r="A332" t="inlineStr">
@@ -4752,6 +5747,9 @@
       <c r="C332" t="n">
         <v>0</v>
       </c>
+      <c r="D332" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="333">
       <c r="A333" t="inlineStr">
@@ -4765,6 +5763,9 @@
       <c r="C333" t="n">
         <v>0</v>
       </c>
+      <c r="D333" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="334">
       <c r="A334" t="inlineStr">
@@ -4778,6 +5779,9 @@
       <c r="C334" t="n">
         <v>0</v>
       </c>
+      <c r="D334" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="335">
       <c r="A335" t="inlineStr">
@@ -4791,6 +5795,9 @@
       <c r="C335" t="n">
         <v>0</v>
       </c>
+      <c r="D335" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="336">
       <c r="A336" t="inlineStr">
@@ -4802,7 +5809,10 @@
         <v>30</v>
       </c>
       <c r="C336" t="n">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="D336" t="n">
+        <v>3.333333333333333</v>
       </c>
     </row>
     <row r="337">
@@ -4817,6 +5827,9 @@
       <c r="C337" t="n">
         <v>0</v>
       </c>
+      <c r="D337" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="338">
       <c r="A338" t="inlineStr">
@@ -4830,6 +5843,9 @@
       <c r="C338" t="n">
         <v>0</v>
       </c>
+      <c r="D338" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="339">
       <c r="A339" t="inlineStr">
@@ -4843,6 +5859,9 @@
       <c r="C339" t="n">
         <v>0</v>
       </c>
+      <c r="D339" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="340">
       <c r="A340" t="inlineStr">
@@ -4856,6 +5875,9 @@
       <c r="C340" t="n">
         <v>0</v>
       </c>
+      <c r="D340" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="341">
       <c r="A341" t="inlineStr">
@@ -4869,6 +5891,9 @@
       <c r="C341" t="n">
         <v>0</v>
       </c>
+      <c r="D341" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="342">
       <c r="A342" t="inlineStr">
@@ -4880,7 +5905,10 @@
         <v>30</v>
       </c>
       <c r="C342" t="n">
-        <v>0</v>
+        <v>9</v>
+      </c>
+      <c r="D342" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="343">
@@ -4895,6 +5923,9 @@
       <c r="C343" t="n">
         <v>0</v>
       </c>
+      <c r="D343" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="344">
       <c r="A344" t="inlineStr">
@@ -4908,6 +5939,9 @@
       <c r="C344" t="n">
         <v>0</v>
       </c>
+      <c r="D344" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="345">
       <c r="A345" t="inlineStr">
@@ -4921,6 +5955,9 @@
       <c r="C345" t="n">
         <v>0</v>
       </c>
+      <c r="D345" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="346">
       <c r="A346" t="inlineStr">
@@ -4932,7 +5969,10 @@
         <v>30</v>
       </c>
       <c r="C346" t="n">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="D346" t="n">
+        <v>3.333333333333333</v>
       </c>
     </row>
     <row r="347">
@@ -4945,7 +5985,10 @@
         <v>50</v>
       </c>
       <c r="C347" t="n">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="D347" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="348">
@@ -4958,7 +6001,10 @@
         <v>74</v>
       </c>
       <c r="C348" t="n">
-        <v>0</v>
+        <v>27</v>
+      </c>
+      <c r="D348" t="n">
+        <v>12.16216216216216</v>
       </c>
     </row>
     <row r="349">
@@ -4971,7 +6017,10 @@
         <v>50</v>
       </c>
       <c r="C349" t="n">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="D349" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="350">
@@ -4986,6 +6035,9 @@
       <c r="C350" t="n">
         <v>0</v>
       </c>
+      <c r="D350" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="351">
       <c r="A351" t="inlineStr">
@@ -4997,7 +6049,10 @@
         <v>61</v>
       </c>
       <c r="C351" t="n">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="D351" t="n">
+        <v>1.639344262295082</v>
       </c>
     </row>
     <row r="352">
@@ -5010,7 +6065,10 @@
         <v>55</v>
       </c>
       <c r="C352" t="n">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="D352" t="n">
+        <v>1.818181818181818</v>
       </c>
     </row>
     <row r="353">
@@ -5025,6 +6083,9 @@
       <c r="C353" t="n">
         <v>0</v>
       </c>
+      <c r="D353" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="354">
       <c r="A354" t="inlineStr">
@@ -5038,6 +6099,9 @@
       <c r="C354" t="n">
         <v>0</v>
       </c>
+      <c r="D354" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="355">
       <c r="A355" t="inlineStr">
@@ -5051,6 +6115,9 @@
       <c r="C355" t="n">
         <v>0</v>
       </c>
+      <c r="D355" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="356">
       <c r="A356" t="inlineStr">
@@ -5062,7 +6129,10 @@
         <v>32</v>
       </c>
       <c r="C356" t="n">
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="D356" t="n">
+        <v>6.25</v>
       </c>
     </row>
     <row r="357">
@@ -5075,7 +6145,10 @@
         <v>30</v>
       </c>
       <c r="C357" t="n">
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="D357" t="n">
+        <v>6.666666666666667</v>
       </c>
     </row>
     <row r="358">
@@ -5088,7 +6161,10 @@
         <v>30</v>
       </c>
       <c r="C358" t="n">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="D358" t="n">
+        <v>3.333333333333333</v>
       </c>
     </row>
     <row r="359">
@@ -5103,6 +6179,9 @@
       <c r="C359" t="n">
         <v>0</v>
       </c>
+      <c r="D359" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="360">
       <c r="A360" t="inlineStr">
@@ -5114,7 +6193,10 @@
         <v>30</v>
       </c>
       <c r="C360" t="n">
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="D360" t="n">
+        <v>6.666666666666667</v>
       </c>
     </row>
     <row r="361">
@@ -5129,6 +6211,9 @@
       <c r="C361" t="n">
         <v>0</v>
       </c>
+      <c r="D361" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="362">
       <c r="A362" t="inlineStr">
@@ -5142,6 +6227,9 @@
       <c r="C362" t="n">
         <v>0</v>
       </c>
+      <c r="D362" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="363">
       <c r="A363" t="inlineStr">
@@ -5155,6 +6243,9 @@
       <c r="C363" t="n">
         <v>0</v>
       </c>
+      <c r="D363" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="364">
       <c r="A364" t="inlineStr">
@@ -5168,6 +6259,9 @@
       <c r="C364" t="n">
         <v>0</v>
       </c>
+      <c r="D364" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="365">
       <c r="A365" t="inlineStr">
@@ -5181,6 +6275,9 @@
       <c r="C365" t="n">
         <v>0</v>
       </c>
+      <c r="D365" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="366">
       <c r="A366" t="inlineStr">
@@ -5194,6 +6291,9 @@
       <c r="C366" t="n">
         <v>0</v>
       </c>
+      <c r="D366" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="367">
       <c r="A367" t="inlineStr">
@@ -5207,6 +6307,9 @@
       <c r="C367" t="n">
         <v>0</v>
       </c>
+      <c r="D367" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="368">
       <c r="A368" t="inlineStr">
@@ -5220,6 +6323,9 @@
       <c r="C368" t="n">
         <v>0</v>
       </c>
+      <c r="D368" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="369">
       <c r="A369" t="inlineStr">
@@ -5233,6 +6339,9 @@
       <c r="C369" t="n">
         <v>0</v>
       </c>
+      <c r="D369" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="370">
       <c r="A370" t="inlineStr">
@@ -5246,6 +6355,9 @@
       <c r="C370" t="n">
         <v>0</v>
       </c>
+      <c r="D370" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="371">
       <c r="A371" t="inlineStr">
@@ -5259,6 +6371,9 @@
       <c r="C371" t="n">
         <v>0</v>
       </c>
+      <c r="D371" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="372">
       <c r="A372" t="inlineStr">
@@ -5272,6 +6387,9 @@
       <c r="C372" t="n">
         <v>0</v>
       </c>
+      <c r="D372" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="373">
       <c r="A373" t="inlineStr">
@@ -5285,6 +6403,9 @@
       <c r="C373" t="n">
         <v>0</v>
       </c>
+      <c r="D373" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="374">
       <c r="A374" t="inlineStr">
@@ -5298,6 +6419,9 @@
       <c r="C374" t="n">
         <v>0</v>
       </c>
+      <c r="D374" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="375">
       <c r="A375" t="inlineStr">
@@ -5311,6 +6435,9 @@
       <c r="C375" t="n">
         <v>0</v>
       </c>
+      <c r="D375" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="376">
       <c r="A376" t="inlineStr">
@@ -5324,6 +6451,9 @@
       <c r="C376" t="n">
         <v>0</v>
       </c>
+      <c r="D376" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="377">
       <c r="A377" t="inlineStr">
@@ -5337,6 +6467,9 @@
       <c r="C377" t="n">
         <v>0</v>
       </c>
+      <c r="D377" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="378">
       <c r="A378" t="inlineStr">
@@ -5348,6 +6481,9 @@
         <v>30</v>
       </c>
       <c r="C378" t="n">
+        <v>0</v>
+      </c>
+      <c r="D378" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>